<commit_message>
added a script that doesn't import functions from another local .py file
</commit_message>
<xml_diff>
--- a/example_JFK_speech/wav2vec2_sf_metadata/transcription_time_log.xlsx
+++ b/example_JFK_speech/wav2vec2_sf_metadata/transcription_time_log.xlsx
@@ -420,7 +420,7 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1615324049.762718</v>
+        <v>1615418222.678129</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -431,7 +431,7 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>1615324058.93181</v>
+        <v>1615418233.622086</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -442,7 +442,7 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>1615324061.769993</v>
+        <v>1615418236.867699</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -453,7 +453,7 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>1615324258.911053</v>
+        <v>1615418486.301492</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -464,7 +464,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>1615324259.0178</v>
+        <v>1615418486.43469</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -475,7 +475,7 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>1615324265.792627</v>
+        <v>1615418493.962464</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -486,7 +486,7 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>1615324265.792627</v>
+        <v>1615418493.962464</v>
       </c>
     </row>
   </sheetData>

</xml_diff>